<commit_message>
First implementation of GraphViewGraphFactory
</commit_message>
<xml_diff>
--- a/implementation/GAns_Projektfortschritt.xlsx
+++ b/implementation/GAns_Projektfortschritt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
   <si>
     <t>objectproperties</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Jonas F + Lucas</t>
   </si>
 </sst>
 </file>
@@ -847,11 +850,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-192108976"/>
-        <c:axId val="-192105712"/>
+        <c:axId val="1397569328"/>
+        <c:axId val="1397562800"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-192108976"/>
+        <c:axId val="1397569328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,14 +894,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-192105712"/>
+        <c:crossAx val="1397562800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-192105712"/>
+        <c:axId val="1397562800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="272"/>
@@ -948,7 +951,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-192108976"/>
+        <c:crossAx val="1397569328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -1835,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G7" s="28">
         <v>0</v>
@@ -2164,7 +2167,7 @@
         <v>33</v>
       </c>
       <c r="G16" s="28">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H16" s="25"/>
     </row>
@@ -2763,7 +2766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2957,7 +2960,7 @@
       </c>
       <c r="C31">
         <f>Daten!D3*(Daten!G3/100)+Daten!D4*(Daten!G4/100)+Daten!D5*(Daten!G5/100)+Daten!D6*(Daten!G6/100)+Daten!D7*(Daten!G7/100)+Daten!D8*(Daten!G8/100)+Daten!D9*(Daten!G9/100)+Daten!D10*(Daten!G10/100)+Daten!D11*(Daten!G11/100)+Daten!D12*(Daten!G12/100)+Daten!D13*(Daten!G13/100)+Daten!D14*(Daten!G14/100)+Daten!D15*(Daten!G15/100)+Daten!D16*(Daten!G16/100)+Daten!D18*(Daten!G18/100)+Daten!D19*(Daten!G19/100)+Daten!D20*(Daten!G20/100)+Daten!D21*(Daten!G21/100)+Daten!D22*(Daten!G22/100)+Daten!D23*(Daten!G23/100)+Daten!D24*(Daten!G24/100)+Daten!D25*(Daten!G25/100)+Daten!D26*(Daten!G26/100)+Daten!D27*(Daten!G27/100)+Daten!D28*(Daten!G28/100)+Daten!D29*(Daten!G29/100)+Daten!D30*(Daten!G30/100)+Daten!D31*(Daten!G31/100)+Daten!D32*(Daten!G32/100)+Daten!D33*(Daten!G33/100)+Daten!D34*(Daten!G34/100)+Daten!D35*(Daten!G35/100)+Daten!D36*(Daten!G36/100)+Daten!D37*(Daten!G37/100)+Daten!D38*(Daten!G38/100)+Daten!D39*(Daten!G39/100)+Daten!D17*(Daten!G17/100)+Daten!D40*(Daten!G40/100)+Daten!D41*(Daten!G41/100)+Daten!D42*(Daten!G42/100)+Daten!D43*(Daten!G43/100)+Daten!D44*(Daten!G44/100)+Daten!D45*(Daten!G45/100)</f>
-        <v>15</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Datum der Fertigstellung
</commit_message>
<xml_diff>
--- a/implementation/GAns_Projektfortschritt.xlsx
+++ b/implementation/GAns_Projektfortschritt.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>objectproperties</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>Jonas F</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>Jonas F + Lucas</t>
@@ -450,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -496,6 +493,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -850,11 +850,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1397569328"/>
-        <c:axId val="1397562800"/>
+        <c:axId val="-1255253152"/>
+        <c:axId val="-1255251520"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1397569328"/>
+        <c:axId val="-1255253152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,14 +894,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1397562800"/>
+        <c:crossAx val="-1255251520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1397562800"/>
+        <c:axId val="-1255251520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="272"/>
@@ -951,7 +951,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1397569328"/>
+        <c:crossAx val="-1255253152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -1839,7 +1839,7 @@
   <dimension ref="B2:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1938,9 @@
       <c r="G5" s="28">
         <v>100</v>
       </c>
-      <c r="H5" s="25"/>
+      <c r="H5" s="25">
+        <v>42544</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -1959,7 +1961,9 @@
       <c r="G6" s="28">
         <v>100</v>
       </c>
-      <c r="H6" s="25"/>
+      <c r="H6" s="25">
+        <v>42544</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -1975,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="28">
         <v>0</v>
@@ -2181,8 +2185,8 @@
       <c r="D17" s="23">
         <v>6</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>71</v>
+      <c r="E17" s="33">
+        <v>1</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>33</v>
@@ -2190,7 +2194,9 @@
       <c r="G17" s="28">
         <v>100</v>
       </c>
-      <c r="H17" s="25"/>
+      <c r="H17" s="25">
+        <v>42544</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">

</xml_diff>

<commit_message>
updated progress and added changes
</commit_message>
<xml_diff>
--- a/implementation/GAns_Projektfortschritt.xlsx
+++ b/implementation/GAns_Projektfortschritt.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\PSEDokumente\implementation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas_000\Documents\Studium\PSE - Visualisierung von Programmgraphen\PSEDokumente\implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
     <sheet name="Auswertung" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -177,9 +177,6 @@
     <t>GraphBuilder-Klassen</t>
   </si>
   <si>
-    <t>Nicolas + Lucas</t>
-  </si>
-  <si>
     <t>Import und Export anstoßen + Dialoge</t>
   </si>
   <si>
@@ -250,12 +247,15 @@
   </si>
   <si>
     <t>Vorraussichtliches Fertigstellungsdatum:</t>
+  </si>
+  <si>
+    <t>Nicolas + Lucas (+Jonas F)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
@@ -609,7 +609,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -651,7 +651,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -686,7 +685,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -695,14 +693,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -711,14 +709,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -727,14 +725,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -743,14 +741,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -759,14 +757,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -775,14 +773,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -791,14 +789,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -807,14 +805,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -823,14 +821,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -839,14 +837,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -855,14 +853,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -871,14 +869,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -887,14 +885,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="13"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -903,14 +901,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="14"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -919,8 +917,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1054,6 +1053,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-2D21-4B87-AA9C-14C8F93AF4E8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1081,7 +1085,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1090,14 +1093,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1106,14 +1109,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1122,14 +1125,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1138,14 +1141,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1154,14 +1157,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1170,14 +1173,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1186,14 +1189,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1202,14 +1205,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1218,14 +1221,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1234,14 +1237,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1250,14 +1253,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001A-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1266,14 +1269,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001B-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1282,14 +1285,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001C-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="13"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1298,14 +1301,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001D-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="14"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1314,8 +1317,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001E-2D21-4B87-AA9C-14C8F93AF4E8}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1422,6 +1426,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001F-2D21-4B87-AA9C-14C8F93AF4E8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1547,7 +1556,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1615,7 +1623,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1690,6 +1698,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1725,6 +1750,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1880,23 +1922,23 @@
   <dimension ref="B2:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875"/>
-    <col min="2" max="2" width="18.140625"/>
-    <col min="3" max="3" width="39.28515625"/>
-    <col min="4" max="4" width="11.7109375"/>
-    <col min="5" max="5" width="7.7109375"/>
+    <col min="1" max="1" width="10.88671875"/>
+    <col min="2" max="2" width="18.109375"/>
+    <col min="3" max="3" width="39.33203125"/>
+    <col min="4" max="4" width="11.6640625"/>
+    <col min="5" max="5" width="7.6640625"/>
     <col min="6" max="6" width="25"/>
-    <col min="7" max="7" width="21.140625"/>
-    <col min="8" max="9" width="24.7109375"/>
-    <col min="10" max="1025" width="10.85546875"/>
+    <col min="7" max="7" width="21.109375"/>
+    <col min="8" max="9" width="24.6640625"/>
+    <col min="10" max="1025" width="10.88671875"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1920,7 +1962,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1942,7 +1984,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1964,7 +2006,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1988,7 +2030,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
@@ -2012,7 +2054,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2036,7 +2078,7 @@
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2058,7 +2100,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
@@ -2082,7 +2124,7 @@
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
@@ -2104,7 +2146,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
@@ -2126,7 +2168,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
@@ -2148,7 +2190,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -2170,7 +2212,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
@@ -2192,7 +2234,7 @@
       <c r="H14" s="12"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
@@ -2216,7 +2258,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>33</v>
       </c>
@@ -2238,7 +2280,7 @@
       <c r="H16" s="12"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>33</v>
       </c>
@@ -2262,7 +2304,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>36</v>
       </c>
@@ -2284,7 +2326,7 @@
       <c r="H18" s="12"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>36</v>
       </c>
@@ -2308,7 +2350,7 @@
       </c>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>33</v>
       </c>
@@ -2330,7 +2372,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
@@ -2352,7 +2394,7 @@
       <c r="H21" s="12"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
@@ -2374,7 +2416,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>41</v>
       </c>
@@ -2396,7 +2438,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
         <v>41</v>
       </c>
@@ -2418,7 +2460,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
@@ -2440,7 +2482,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>41</v>
       </c>
@@ -2462,7 +2504,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
@@ -2484,7 +2526,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
@@ -2506,7 +2548,7 @@
       <c r="H28" s="12"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>41</v>
       </c>
@@ -2528,7 +2570,7 @@
       <c r="H29" s="12"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>41</v>
       </c>
@@ -2542,20 +2584,20 @@
         <v>2</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="G30" s="11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="17">
         <v>5</v>
@@ -2564,7 +2606,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" s="11">
         <v>100</v>
@@ -2572,12 +2614,12 @@
       <c r="H31" s="12"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="17">
         <v>6</v>
@@ -2594,9 +2636,9 @@
       <c r="H32" s="12"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>14</v>
@@ -2608,20 +2650,20 @@
         <v>2</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" s="11">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="17">
         <v>10</v>
@@ -2636,12 +2678,12 @@
       <c r="H34" s="12"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="17">
         <v>10</v>
@@ -2656,12 +2698,12 @@
       <c r="H35" s="12"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36" s="17">
         <v>6</v>
@@ -2676,12 +2718,12 @@
       <c r="H36" s="12"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" s="17">
         <v>13</v>
@@ -2696,12 +2738,12 @@
       <c r="H37" s="12"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" s="17">
         <v>13</v>
@@ -2716,12 +2758,12 @@
       <c r="H38" s="12"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="17">
         <v>10</v>
@@ -2736,12 +2778,12 @@
       <c r="H39" s="12"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D40" s="17">
         <v>7</v>
@@ -2756,12 +2798,12 @@
       <c r="H40" s="12"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D41" s="17">
         <v>4</v>
@@ -2776,12 +2818,12 @@
       <c r="H41" s="12"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" s="17">
         <v>4</v>
@@ -2796,12 +2838,12 @@
       <c r="H42" s="12"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43" s="17">
         <v>4</v>
@@ -2816,12 +2858,12 @@
       <c r="H43" s="12"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" s="17">
         <v>4</v>
@@ -2836,9 +2878,9 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>14</v>
@@ -2867,22 +2909,22 @@
   <dimension ref="B1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875"/>
-    <col min="2" max="2" width="39.28515625"/>
-    <col min="3" max="1025" width="10.85546875"/>
+    <col min="1" max="1" width="10.88671875"/>
+    <col min="2" max="2" width="39.33203125"/>
+    <col min="3" max="1025" width="10.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:19" x14ac:dyDescent="0.3">
       <c r="G1" s="27"/>
     </row>
-    <row r="5" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="27">
         <v>42542</v>
@@ -2930,9 +2972,9 @@
         <v>42570</v>
       </c>
     </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="28">
         <v>0</v>
@@ -2994,9 +3036,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="28">
         <v>0</v>
@@ -3026,39 +3068,39 @@
       <c r="R7" s="28"/>
       <c r="S7" s="28"/>
     </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D8" s="29"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="30">
         <f>Daten!D3+Daten!D4+Daten!D5+Daten!D6+Daten!D7+Daten!D8+Daten!D9+Daten!D10+Daten!D11+Daten!D12+Daten!D13+Daten!D14+Daten!D15+Daten!D16+Daten!D18+Daten!D19+Daten!D20+Daten!D21+Daten!D22+Daten!D23+Daten!D24+Daten!D25+Daten!D26+Daten!D27+Daten!D28+Daten!D29+Daten!D30+Daten!D31+Daten!D32+Daten!D33+Daten!D34+Daten!D35+Daten!D36+Daten!D37+Daten!D38+Daten!D39+Daten!D17+Daten!D40+Daten!D41+Daten!D42+Daten!D43+Daten!D44+Daten!D45</f>
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31">
         <f>Daten!D3*(Daten!G3/100)+Daten!D4*(Daten!G4/100)+Daten!D5*(Daten!G5/100)+Daten!D6*(Daten!G6/100)+Daten!D7*(Daten!G7/100)+Daten!D8*(Daten!G8/100)+Daten!D9*(Daten!G9/100)+Daten!D10*(Daten!G10/100)+Daten!D11*(Daten!G11/100)+Daten!D12*(Daten!G12/100)+Daten!D13*(Daten!G13/100)+Daten!D14*(Daten!G14/100)+Daten!D15*(Daten!G15/100)+Daten!D16*(Daten!G16/100)+Daten!D18*(Daten!G18/100)+Daten!D19*(Daten!G19/100)+Daten!D20*(Daten!G20/100)+Daten!D21*(Daten!G21/100)+Daten!D22*(Daten!G22/100)+Daten!D23*(Daten!G23/100)+Daten!D24*(Daten!G24/100)+Daten!D25*(Daten!G25/100)+Daten!D26*(Daten!G26/100)+Daten!D27*(Daten!G27/100)+Daten!D28*(Daten!G28/100)+Daten!D29*(Daten!G29/100)+Daten!D30*(Daten!G30/100)+Daten!D31*(Daten!G31/100)+Daten!D32*(Daten!G32/100)+Daten!D33*(Daten!G33/100)+Daten!D34*(Daten!G34/100)+Daten!D35*(Daten!G35/100)+Daten!D36*(Daten!G36/100)+Daten!D37*(Daten!G37/100)+Daten!D38*(Daten!G38/100)+Daten!D39*(Daten!G39/100)+Daten!D17*(Daten!G17/100)+Daten!D40*(Daten!G40/100)+Daten!D41*(Daten!G41/100)+Daten!D42*(Daten!G42/100)+Daten!D43*(Daten!G43/100)+Daten!D44*(Daten!G44/100)+Daten!D45*(Daten!G45/100)</f>
-        <v>87.509999999999991</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+        <v>97.399999999999991</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="30">
         <f>C30/((5*16)/7)</f>
         <v>23.8</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="27">
         <f>E5+C32</f>

</xml_diff>

<commit_message>
anderungen zum entwurf und fortschritt angepasst
</commit_message>
<xml_diff>
--- a/implementation/GAns_Projektfortschritt.xlsx
+++ b/implementation/GAns_Projektfortschritt.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\PSEDokumente\implementation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas_000\Documents\Studium\PSE - Visualisierung von Programmgraphen\PSEDokumente\implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7830" tabRatio="845"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7836" tabRatio="845"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
     <sheet name="Auswertung" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
@@ -610,7 +610,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -649,7 +649,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -755,7 +754,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -883,6 +881,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-473E-44F8-AB2C-99D448F10D07}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -954,7 +957,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1067,6 +1069,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-473E-44F8-AB2C-99D448F10D07}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="t"/>
@@ -1198,7 +1205,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1844,7 +1850,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1919,6 +1925,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1954,6 +1977,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2108,24 +2148,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375"/>
-    <col min="2" max="2" width="17.85546875"/>
-    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125"/>
-    <col min="5" max="5" width="7.5703125"/>
-    <col min="6" max="6" width="24.85546875"/>
-    <col min="7" max="7" width="20.85546875"/>
-    <col min="8" max="9" width="24.7109375"/>
-    <col min="10" max="1025" width="10.7109375"/>
+    <col min="1" max="1" width="10.6640625"/>
+    <col min="2" max="2" width="17.88671875"/>
+    <col min="3" max="3" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625"/>
+    <col min="5" max="5" width="7.5546875"/>
+    <col min="6" max="6" width="24.88671875"/>
+    <col min="7" max="7" width="20.88671875"/>
+    <col min="8" max="9" width="24.6640625"/>
+    <col min="10" max="1025" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2149,7 +2189,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -2173,7 +2213,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
@@ -2195,7 +2235,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
@@ -2219,7 +2259,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
@@ -2243,7 +2283,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2267,7 +2307,7 @@
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2289,7 +2329,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
@@ -2313,7 +2353,7 @@
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
@@ -2330,12 +2370,12 @@
         <v>25</v>
       </c>
       <c r="G10" s="11">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
@@ -2357,7 +2397,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
@@ -2379,7 +2419,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -2403,7 +2443,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
@@ -2427,7 +2467,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
@@ -2451,7 +2491,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>33</v>
       </c>
@@ -2473,7 +2513,7 @@
       <c r="H16" s="12"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>33</v>
       </c>
@@ -2497,7 +2537,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>36</v>
       </c>
@@ -2519,7 +2559,7 @@
       <c r="H18" s="12"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>36</v>
       </c>
@@ -2543,7 +2583,7 @@
       </c>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>33</v>
       </c>
@@ -2565,7 +2605,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
@@ -2589,7 +2629,7 @@
       </c>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
@@ -2613,7 +2653,7 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>41</v>
       </c>
@@ -2635,7 +2675,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
         <v>41</v>
       </c>
@@ -2657,7 +2697,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
@@ -2679,7 +2719,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>41</v>
       </c>
@@ -2701,7 +2741,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
@@ -2723,7 +2763,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
@@ -2745,7 +2785,7 @@
       <c r="H28" s="12"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>41</v>
       </c>
@@ -2767,7 +2807,7 @@
       <c r="H29" s="12"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>41</v>
       </c>
@@ -2789,7 +2829,7 @@
       <c r="H30" s="12"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>33</v>
       </c>
@@ -2813,7 +2853,7 @@
       </c>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
         <v>33</v>
       </c>
@@ -2837,7 +2877,7 @@
       </c>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>54</v>
       </c>
@@ -2861,7 +2901,7 @@
       </c>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>26</v>
       </c>
@@ -2883,7 +2923,7 @@
       <c r="H34" s="12"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>26</v>
       </c>
@@ -2905,7 +2945,7 @@
       <c r="H35" s="12"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
         <v>41</v>
       </c>
@@ -2927,7 +2967,7 @@
       <c r="H36" s="12"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>41</v>
       </c>
@@ -2949,7 +2989,7 @@
       <c r="H37" s="12"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
         <v>41</v>
       </c>
@@ -2971,7 +3011,7 @@
       <c r="H38" s="12"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>33</v>
       </c>
@@ -2993,7 +3033,7 @@
       <c r="H39" s="12"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
         <v>36</v>
       </c>
@@ -3015,7 +3055,7 @@
       <c r="H40" s="12"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
         <v>36</v>
       </c>
@@ -3037,7 +3077,7 @@
       <c r="H41" s="12"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
         <v>33</v>
       </c>
@@ -3059,7 +3099,7 @@
       <c r="H42" s="12"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
         <v>33</v>
       </c>
@@ -3081,7 +3121,7 @@
       <c r="H43" s="12"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
         <v>33</v>
       </c>
@@ -3103,7 +3143,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="20" t="s">
         <v>66</v>
       </c>
@@ -3120,7 +3160,7 @@
         <v>55</v>
       </c>
       <c r="G45" s="25">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H45" s="26"/>
       <c r="I45" s="13"/>
@@ -3139,17 +3179,17 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375"/>
-    <col min="2" max="2" width="39.140625"/>
-    <col min="3" max="1025" width="10.7109375"/>
+    <col min="1" max="1" width="10.6640625"/>
+    <col min="2" max="2" width="39.109375"/>
+    <col min="3" max="1025" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:19" x14ac:dyDescent="0.3">
       <c r="G1" s="27"/>
     </row>
-    <row r="5" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>67</v>
       </c>
@@ -3199,7 +3239,7 @@
         <v>42570</v>
       </c>
     </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>68</v>
       </c>
@@ -3263,7 +3303,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>69</v>
       </c>
@@ -3303,10 +3343,10 @@
       <c r="R7" s="28"/>
       <c r="S7" s="28"/>
     </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D8" s="29"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>70</v>
       </c>
@@ -3315,16 +3355,16 @@
         <v>263</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>71</v>
       </c>
       <c r="C31">
         <f>Daten!D3*(Daten!G3/100)+Daten!D4*(Daten!G4/100)+Daten!D5*(Daten!G5/100)+Daten!D6*(Daten!G6/100)+Daten!D7*(Daten!G7/100)+Daten!D8*(Daten!G8/100)+Daten!D9*(Daten!G9/100)+Daten!D10*(Daten!G10/100)+Daten!D11*(Daten!G11/100)+Daten!D12*(Daten!G12/100)+Daten!D13*(Daten!G13/100)+Daten!D14*(Daten!G14/100)+Daten!D15*(Daten!G15/100)+Daten!D16*(Daten!G16/100)+Daten!D18*(Daten!G18/100)+Daten!D19*(Daten!G19/100)+Daten!D20*(Daten!G20/100)+Daten!D21*(Daten!G21/100)+Daten!D22*(Daten!G22/100)+Daten!D23*(Daten!G23/100)+Daten!D24*(Daten!G24/100)+Daten!D25*(Daten!G25/100)+Daten!D26*(Daten!G26/100)+Daten!D27*(Daten!G27/100)+Daten!D28*(Daten!G28/100)+Daten!D29*(Daten!G29/100)+Daten!D30*(Daten!G30/100)+Daten!D31*(Daten!G31/100)+Daten!D32*(Daten!G32/100)+Daten!D33*(Daten!G33/100)+Daten!D34*(Daten!G34/100)+Daten!D35*(Daten!G35/100)+Daten!D36*(Daten!G36/100)+Daten!D37*(Daten!G37/100)+Daten!D38*(Daten!G38/100)+Daten!D39*(Daten!G39/100)+Daten!D17*(Daten!G17/100)+Daten!D40*(Daten!G40/100)+Daten!D41*(Daten!G41/100)+Daten!D42*(Daten!G42/100)+Daten!D43*(Daten!G43/100)+Daten!D44*(Daten!G44/100)+Daten!D45*(Daten!G45/100)</f>
-        <v>194.44999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+        <v>199.04999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -3333,7 +3373,7 @@
         <v>23.012499999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>73</v>
       </c>

</xml_diff>